<commit_message>
update maven cmd run tescase
</commit_message>
<xml_diff>
--- a/data/login.xlsx
+++ b/data/login.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\eclipse_WS\tester\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E1D5D8-7D88-40A4-AC14-B483CA8C804F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{501AF69C-7E8C-4DE7-86E0-CE3ABB6A8D58}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-23148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -33,38 +33,36 @@
     <t>Testname</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
     <t>Result</t>
   </si>
   <si>
     <t>Error</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Alert</t>
-  </si>
-  <si>
-    <t>Password không được để trống</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>Hoàng dl</t>
+    <t xml:space="preserve">The email address or mobile number you entered isn't connected to an account. </t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,45 +71,51 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,12 +124,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.249977111117893"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -134,76 +198,132 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+  <cellXfs count="8">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="8" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="12" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="16" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="20" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -220,10 +340,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -258,7 +378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -293,7 +413,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -387,21 +507,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -418,7 +538,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -470,91 +590,67 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="70.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="47.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix change test status skip to pass
</commit_message>
<xml_diff>
--- a/data/login.xlsx
+++ b/data/login.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +114,20 @@
       <b val="true"/>
       <color indexed="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +200,28 @@
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -305,11 +337,47 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -317,7 +385,9 @@
     <xf applyBorder="true" applyFill="true" borderId="12" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="16" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="20" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="24" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="28" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="32" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -646,7 +716,7 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create sutiefile run all testcase
</commit_message>
<xml_diff>
--- a/data/login.xlsx
+++ b/data/login.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +126,32 @@
       <b val="true"/>
       <color indexed="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +244,48 @@
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -373,11 +437,83 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -387,7 +523,11 @@
     <xf applyBorder="true" applyFill="true" borderId="20" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="24" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="28" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="32" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="32" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="36" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="40" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="44" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="48" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -716,7 +856,7 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change eclipse to intellij
</commit_message>
<xml_diff>
--- a/data/login.xlsx
+++ b/data/login.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +162,44 @@
       <b val="true"/>
       <color indexed="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="31">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,8 +352,68 @@
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="57">
+  <borders count="81">
     <border>
       <left/>
       <right/>
@@ -577,11 +673,119 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -597,7 +801,13 @@
     <xf applyBorder="true" applyFill="true" borderId="44" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="48" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="52" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="56" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="56" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="60" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="64" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="68" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="72" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="76" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="80" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -926,7 +1136,7 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="21" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>